<commit_message>
vu update file thuc_hanh_git
</commit_message>
<xml_diff>
--- a/git_learn/thuc_hanh_git.xlsx
+++ b/git_learn/thuc_hanh_git.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t xml:space="preserve">Câu lệnh</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t xml:space="preserve">Thực hiện chuyển các commit đã thực hiện ở branch my-branch sang branch master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git checkout -b vu-branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạo branch mới có tên vu-branch. Khi đó các commit có trên branch master cũng sẽ có trên my-branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thuc hien update file thuc_hanh_git, luu file</t>
   </si>
   <si>
     <t xml:space="preserve">Hiện tại branch master mới chỉ có 1 commit add index.html file</t>
@@ -457,18 +466,18 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>340</xdr:row>
+      <xdr:row>352</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>153000</xdr:colOff>
-      <xdr:row>348</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121680</xdr:colOff>
+      <xdr:row>364</xdr:row>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 21" descr=""/>
+        <xdr:cNvPr id="2" name="Image 22" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -477,44 +486,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="67541400"/>
-          <a:ext cx="7040520" cy="1681920"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>352</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>121680</xdr:colOff>
-      <xdr:row>365</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 22" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6604920" y="69977880"/>
+          <a:off x="6604920" y="69922080"/>
           <a:ext cx="7824240" cy="2695680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -542,16 +514,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 23" descr=""/>
+        <xdr:cNvPr id="3" name="Image 23" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip r:embed="rId4"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="73557360"/>
+          <a:off x="6604920" y="73652040"/>
           <a:ext cx="5591160" cy="1414080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -569,26 +541,26 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>380</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>534960</xdr:colOff>
-      <xdr:row>393</xdr:row>
-      <xdr:rowOff>191160</xdr:rowOff>
+      <xdr:row>394</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 24" descr=""/>
+        <xdr:cNvPr id="4" name="Image 24" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
+        <a:blip r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="75462840"/>
+          <a:off x="6604920" y="75557520"/>
           <a:ext cx="9052920" cy="2666880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -606,7 +578,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>398</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -616,16 +588,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 25" descr=""/>
+        <xdr:cNvPr id="5" name="Image 25" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <a:blip r:embed="rId6"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="78891840"/>
+          <a:off x="6604920" y="78986520"/>
           <a:ext cx="9141840" cy="2226960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -643,26 +615,26 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>413</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>95760</xdr:colOff>
       <xdr:row>421</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 26" descr=""/>
+        <xdr:cNvPr id="6" name="Image 26" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <a:blip r:embed="rId7"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="81748800"/>
+          <a:off x="6604920" y="81843120"/>
           <a:ext cx="6167880" cy="1681920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -680,26 +652,26 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>425</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>202680</xdr:colOff>
       <xdr:row>427</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 27" descr=""/>
+        <xdr:cNvPr id="7" name="Image 27" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
+        <a:blip r:embed="rId8"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="84185280"/>
+          <a:off x="6604920" y="84279600"/>
           <a:ext cx="7090200" cy="630000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -727,16 +699,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 28" descr=""/>
+        <xdr:cNvPr id="8" name="Image 28" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10"/>
+        <a:blip r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="85287960"/>
+          <a:off x="6604920" y="85382640"/>
           <a:ext cx="8180280" cy="620640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -764,16 +736,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 29" descr=""/>
+        <xdr:cNvPr id="9" name="Image 29" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11"/>
+        <a:blip r:embed="rId10"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="86391360"/>
+          <a:off x="6604920" y="86486040"/>
           <a:ext cx="6177600" cy="4149000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -801,16 +773,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Image 30" descr=""/>
+        <xdr:cNvPr id="10" name="Image 30" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
+        <a:blip r:embed="rId11"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="91535040"/>
+          <a:off x="6604920" y="91629720"/>
           <a:ext cx="6414840" cy="1375920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -838,16 +810,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Image 31" descr=""/>
+        <xdr:cNvPr id="11" name="Image 31" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13"/>
+        <a:blip r:embed="rId12"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="93439440"/>
+          <a:off x="6604920" y="93534120"/>
           <a:ext cx="5729760" cy="1548000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -875,16 +847,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Image 32" descr=""/>
+        <xdr:cNvPr id="12" name="Image 32" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14"/>
+        <a:blip r:embed="rId13"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="95685840"/>
+          <a:off x="6604920" y="95780520"/>
           <a:ext cx="9300240" cy="3393720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -902,7 +874,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>505</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
@@ -912,16 +884,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Image 33" descr=""/>
+        <xdr:cNvPr id="13" name="Image 33" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15"/>
+        <a:blip r:embed="rId14"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="99877320"/>
+          <a:off x="6604920" y="99972000"/>
           <a:ext cx="9043200" cy="2638080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -949,11 +921,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Image 8" descr=""/>
+        <xdr:cNvPr id="14" name="Image 8" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16"/>
+        <a:blip r:embed="rId15"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -986,11 +958,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Image 1" descr=""/>
+        <xdr:cNvPr id="15" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17"/>
+        <a:blip r:embed="rId16"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1023,11 +995,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Image 3" descr=""/>
+        <xdr:cNvPr id="16" name="Image 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18"/>
+        <a:blip r:embed="rId17"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1060,11 +1032,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Image 4" descr=""/>
+        <xdr:cNvPr id="17" name="Image 4" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19"/>
+        <a:blip r:embed="rId18"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1097,11 +1069,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Image 5" descr=""/>
+        <xdr:cNvPr id="18" name="Image 5" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20"/>
+        <a:blip r:embed="rId19"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1134,11 +1106,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Image 6" descr=""/>
+        <xdr:cNvPr id="19" name="Image 6" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21"/>
+        <a:blip r:embed="rId20"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1171,11 +1143,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Image 10" descr=""/>
+        <xdr:cNvPr id="20" name="Image 10" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22"/>
+        <a:blip r:embed="rId21"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1208,11 +1180,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Image 7" descr=""/>
+        <xdr:cNvPr id="21" name="Image 7" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23"/>
+        <a:blip r:embed="rId22"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1245,11 +1217,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Image 11" descr=""/>
+        <xdr:cNvPr id="22" name="Image 11" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24"/>
+        <a:blip r:embed="rId23"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1282,11 +1254,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Image 12" descr=""/>
+        <xdr:cNvPr id="23" name="Image 12" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25"/>
+        <a:blip r:embed="rId24"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1319,11 +1291,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Image 13" descr=""/>
+        <xdr:cNvPr id="24" name="Image 13" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26"/>
+        <a:blip r:embed="rId25"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1356,11 +1328,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Image 14" descr=""/>
+        <xdr:cNvPr id="25" name="Image 14" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27"/>
+        <a:blip r:embed="rId26"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1393,11 +1365,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Image 15" descr=""/>
+        <xdr:cNvPr id="26" name="Image 15" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28"/>
+        <a:blip r:embed="rId27"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1430,11 +1402,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Image 16" descr=""/>
+        <xdr:cNvPr id="27" name="Image 16" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29"/>
+        <a:blip r:embed="rId28"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -1467,7 +1439,44 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Image 17" descr=""/>
+        <xdr:cNvPr id="28" name="Image 17" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId29"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604560" y="62330760"/>
+          <a:ext cx="6975720" cy="1230840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>323640</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>34200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Image 18" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1476,8 +1485,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604560" y="62330760"/>
-          <a:ext cx="6975720" cy="1230840"/>
+          <a:off x="6604560" y="63798840"/>
+          <a:ext cx="7211520" cy="2442960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>313920</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>117720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Image 19" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId31"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604560" y="66778920"/>
+          <a:ext cx="7201800" cy="1545840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1499,8 +1545,8 @@
   </sheetPr>
   <dimension ref="A1:C524"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A305" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A322" activeCellId="0" sqref="A322:B322"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A336" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B345" activeCellId="0" sqref="B345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2923,9 +2969,13 @@
       <c r="A336" s="2"/>
       <c r="B336" s="2"/>
     </row>
-    <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="2"/>
-      <c r="B337" s="2"/>
+    <row r="337" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2"/>
@@ -2939,20 +2989,6 @@
       <c r="A340" s="2"/>
       <c r="B340" s="2"/>
     </row>
-    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B341" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="342" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="2"/>
-      <c r="B342" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2"/>
       <c r="B343" s="2"/>
@@ -2963,7 +2999,9 @@
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2"/>
-      <c r="B345" s="2"/>
+      <c r="B345" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2"/>
@@ -2990,12 +3028,18 @@
       <c r="B351" s="2"/>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="2"/>
-      <c r="B352" s="2"/>
-    </row>
-    <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2"/>
-      <c r="B353" s="2"/>
+      <c r="B353" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="354" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
@@ -3126,7 +3170,7 @@
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2"/>
       <c r="B383" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,7 +3240,7 @@
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2"/>
       <c r="B400" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3253,10 +3297,10 @@
     </row>
     <row r="414" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,10 +3349,10 @@
     </row>
     <row r="426" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,18 +3373,18 @@
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3360,7 +3404,7 @@
         <v>21</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3480,7 +3524,7 @@
         <v>58</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3576,7 +3620,7 @@
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2"/>
       <c r="B486" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,12 +3706,12 @@
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2"/>
       <c r="B507" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create file .gitkeep on folder networking_learn
</commit_message>
<xml_diff>
--- a/git_learn/thuc_hanh_git.xlsx
+++ b/git_learn/thuc_hanh_git.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
   <si>
     <t xml:space="preserve">Câu lệnh</t>
   </si>
@@ -243,6 +243,57 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/vuxquang89/git_demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git log –oneline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiển thị các commit thu gọn bao gồm mã băm và nội dung commit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git reset hash_code_commit [--hard]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trở lại lần commit tương ứng với mã băm, nếu thêm --hard: nó sẽ xóa các thay đổi trong tệp kể từ lần xác nhận trước đó.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git restore .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">để phục hồi các file của thư mục làm việc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git stash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lưu lại công việc đang làm tại branch hiện tại trước khi chuyển sang branch khác</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git stash pop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bật lại các thay đổi đang hoạt động trước đó </t>
+  </si>
+  <si>
+    <t xml:space="preserve">git pull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sẽ tải xuống nội dung và cố gắng thay đổi trạng thái của Local repository cho phù hợp với nội dung đó</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git fetch &lt;remote&gt; &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hỉ tải xuống nội dung từ Remote repository mà không làm thay đổi trạng thái của Local repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git fetch origin &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">touch networking_learn/.gitkeep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tạo file ẩn trong thư mục networking_learn</t>
   </si>
 </sst>
 </file>
@@ -337,7 +388,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -356,6 +407,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -377,11 +432,11 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>410400</xdr:colOff>
+      <xdr:colOff>410040</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
@@ -396,8 +451,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="2116080"/>
-          <a:ext cx="7297920" cy="1299600"/>
+          <a:off x="6604920" y="2116440"/>
+          <a:ext cx="7302600" cy="1299240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -414,11 +469,11 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>20160</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>512640</xdr:colOff>
+      <xdr:colOff>512280</xdr:colOff>
       <xdr:row>155</xdr:row>
       <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
@@ -433,45 +488,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6624720" y="29822040"/>
-          <a:ext cx="5749560" cy="1299600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>254</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>26280</xdr:colOff>
-      <xdr:row>267</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 15" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6604920" y="50583960"/>
-          <a:ext cx="6098400" cy="2609640"/>
+          <a:off x="6624720" y="29822400"/>
+          <a:ext cx="5751720" cy="1299240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -492,23 +510,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>115560</xdr:colOff>
+      <xdr:colOff>115200</xdr:colOff>
       <xdr:row>281</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 16" descr=""/>
+        <xdr:cNvPr id="2" name="Image 16" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="53821800"/>
-          <a:ext cx="6187680" cy="2303640"/>
+          <a:ext cx="6190920" cy="2303280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -529,23 +547,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>402120</xdr:colOff>
+      <xdr:colOff>401760</xdr:colOff>
       <xdr:row>298</xdr:row>
-      <xdr:rowOff>68400</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 17" descr=""/>
+        <xdr:cNvPr id="3" name="Image 17" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip r:embed="rId4"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="56991960"/>
-          <a:ext cx="6474240" cy="2504160"/>
+          <a:ext cx="6477480" cy="2503800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -562,27 +580,27 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>303</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>346320</xdr:colOff>
+      <xdr:colOff>345960</xdr:colOff>
       <xdr:row>312</xdr:row>
       <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 18" descr=""/>
+        <xdr:cNvPr id="4" name="Image 18" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
+        <a:blip r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="60381000"/>
-          <a:ext cx="4787640" cy="1892160"/>
+          <a:off x="6604920" y="60381360"/>
+          <a:ext cx="4788720" cy="1891800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -603,23 +621,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>384120</xdr:colOff>
+      <xdr:colOff>383760</xdr:colOff>
       <xdr:row>322</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 19" descr=""/>
+        <xdr:cNvPr id="5" name="Image 19" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <a:blip r:embed="rId6"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="63007560"/>
-          <a:ext cx="5640840" cy="1509840"/>
+          <a:ext cx="5643000" cy="1509480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -640,23 +658,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>174600</xdr:colOff>
+      <xdr:colOff>174240</xdr:colOff>
       <xdr:row>336</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 20" descr=""/>
+        <xdr:cNvPr id="6" name="Image 20" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <a:blip r:embed="rId7"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="65404440"/>
-          <a:ext cx="6246720" cy="1882800"/>
+          <a:ext cx="6249960" cy="1882440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,23 +695,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>153000</xdr:colOff>
+      <xdr:colOff>152640</xdr:colOff>
       <xdr:row>348</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 21" descr=""/>
+        <xdr:cNvPr id="7" name="Image 21" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
+        <a:blip r:embed="rId8"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="67880520"/>
-          <a:ext cx="7040520" cy="1681920"/>
+          <a:ext cx="7045200" cy="1681560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -714,23 +732,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>121680</xdr:colOff>
+      <xdr:colOff>121320</xdr:colOff>
       <xdr:row>365</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 22" descr=""/>
+        <xdr:cNvPr id="8" name="Image 22" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10"/>
+        <a:blip r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="70317000"/>
-          <a:ext cx="7824240" cy="2695680"/>
+          <a:ext cx="7830360" cy="2695320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -751,23 +769,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>334080</xdr:colOff>
       <xdr:row>377</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 23" descr=""/>
+        <xdr:cNvPr id="9" name="Image 23" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11"/>
+        <a:blip r:embed="rId10"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="73896480"/>
-          <a:ext cx="5591160" cy="1414080"/>
+          <a:ext cx="5593320" cy="1413720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,27 +802,27 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>380</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>534960</xdr:colOff>
+      <xdr:colOff>534600</xdr:colOff>
       <xdr:row>393</xdr:row>
       <xdr:rowOff>191160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Image 24" descr=""/>
+        <xdr:cNvPr id="10" name="Image 24" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
+        <a:blip r:embed="rId11"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="75801960"/>
-          <a:ext cx="9052920" cy="2666880"/>
+          <a:off x="6604920" y="75802320"/>
+          <a:ext cx="9060120" cy="2666520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -821,27 +839,27 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>398</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>623880</xdr:colOff>
+      <xdr:colOff>623520</xdr:colOff>
       <xdr:row>409</xdr:row>
       <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Image 25" descr=""/>
+        <xdr:cNvPr id="11" name="Image 25" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13"/>
+        <a:blip r:embed="rId12"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="79230960"/>
-          <a:ext cx="9141840" cy="2226960"/>
+          <a:off x="6604920" y="79231320"/>
+          <a:ext cx="9149040" cy="2226600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -862,23 +880,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>95760</xdr:colOff>
+      <xdr:colOff>95400</xdr:colOff>
       <xdr:row>421</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Image 26" descr=""/>
+        <xdr:cNvPr id="12" name="Image 26" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14"/>
+        <a:blip r:embed="rId13"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="82087560"/>
-          <a:ext cx="6167880" cy="1681920"/>
+          <a:ext cx="6171120" cy="1681560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -899,23 +917,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>202680</xdr:colOff>
+      <xdr:colOff>202320</xdr:colOff>
       <xdr:row>427</xdr:row>
-      <xdr:rowOff>98640</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Image 27" descr=""/>
+        <xdr:cNvPr id="13" name="Image 27" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15"/>
+        <a:blip r:embed="rId14"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="84524040"/>
-          <a:ext cx="7090200" cy="630000"/>
+          <a:ext cx="7094880" cy="629640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -936,23 +954,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>477720</xdr:colOff>
+      <xdr:colOff>477360</xdr:colOff>
       <xdr:row>432</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Image 28" descr=""/>
+        <xdr:cNvPr id="14" name="Image 28" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16"/>
+        <a:blip r:embed="rId15"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="85627080"/>
-          <a:ext cx="8180280" cy="620640"/>
+          <a:ext cx="8186400" cy="620280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -973,23 +991,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>105480</xdr:colOff>
+      <xdr:colOff>105120</xdr:colOff>
       <xdr:row>456</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Image 29" descr=""/>
+        <xdr:cNvPr id="15" name="Image 29" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17"/>
+        <a:blip r:embed="rId16"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="86730480"/>
-          <a:ext cx="6177600" cy="4149000"/>
+          <a:ext cx="6180840" cy="4148640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1006,27 +1024,27 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>462</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>342720</xdr:colOff>
+      <xdr:colOff>342360</xdr:colOff>
       <xdr:row>469</xdr:row>
       <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Image 30" descr=""/>
+        <xdr:cNvPr id="16" name="Image 30" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18"/>
+        <a:blip r:embed="rId17"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="91874160"/>
-          <a:ext cx="6414840" cy="1375920"/>
+          <a:off x="6604920" y="91874520"/>
+          <a:ext cx="6418080" cy="1375560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1047,23 +1065,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>473040</xdr:colOff>
+      <xdr:colOff>472680</xdr:colOff>
       <xdr:row>479</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Image 31" descr=""/>
+        <xdr:cNvPr id="17" name="Image 31" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19"/>
+        <a:blip r:embed="rId18"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="93778560"/>
-          <a:ext cx="5729760" cy="1548000"/>
+          <a:ext cx="5731920" cy="1547640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1084,23 +1102,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>782280</xdr:colOff>
+      <xdr:colOff>781920</xdr:colOff>
       <xdr:row>500</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Image 32" descr=""/>
+        <xdr:cNvPr id="18" name="Image 32" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20"/>
+        <a:blip r:embed="rId19"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604920" y="96024960"/>
-          <a:ext cx="9300240" cy="3393720"/>
+          <a:ext cx="9307440" cy="3393360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1117,27 +1135,27 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>505</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>525240</xdr:colOff>
+      <xdr:colOff>524880</xdr:colOff>
       <xdr:row>520</xdr:row>
       <xdr:rowOff>144720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Image 33" descr=""/>
+        <xdr:cNvPr id="19" name="Image 33" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21"/>
+        <a:blip r:embed="rId20"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604920" y="100216440"/>
-          <a:ext cx="9043200" cy="2638080"/>
+          <a:off x="6604920" y="100216800"/>
+          <a:ext cx="9050400" cy="2637720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1158,23 +1176,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>439560</xdr:colOff>
+      <xdr:colOff>439200</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:rowOff>171000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Image 8" descr=""/>
+        <xdr:cNvPr id="20" name="Image 8" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22"/>
+        <a:blip r:embed="rId21"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6633720" y="240480"/>
-          <a:ext cx="7298280" cy="1665000"/>
+          <a:ext cx="7302960" cy="1664640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1195,23 +1213,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>391320</xdr:colOff>
+      <xdr:colOff>390960</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>14400</xdr:rowOff>
+      <xdr:rowOff>14040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Image 1" descr=""/>
+        <xdr:cNvPr id="21" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23"/>
+        <a:blip r:embed="rId22"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6614640" y="4320720"/>
-          <a:ext cx="7269120" cy="4818600"/>
+          <a:ext cx="7273800" cy="4818240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1232,23 +1250,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>342000</xdr:colOff>
+      <xdr:colOff>341640</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>51840</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Image 3" descr=""/>
+        <xdr:cNvPr id="22" name="Image 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24"/>
+        <a:blip r:embed="rId23"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604560" y="10077120"/>
-          <a:ext cx="7229880" cy="1316160"/>
+          <a:ext cx="7234560" cy="1315800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1269,23 +1287,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>351720</xdr:colOff>
+      <xdr:colOff>351360</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>180000</xdr:rowOff>
+      <xdr:rowOff>179640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Image 4" descr=""/>
+        <xdr:cNvPr id="23" name="Image 4" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25"/>
+        <a:blip r:embed="rId24"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604560" y="27480240"/>
-          <a:ext cx="7239600" cy="3949920"/>
+          <a:ext cx="7244280" cy="3949560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,23 +1324,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>381240</xdr:colOff>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>183</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Image 5" descr=""/>
+        <xdr:cNvPr id="24" name="Image 5" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26"/>
+        <a:blip r:embed="rId25"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604560" y="32232600"/>
-          <a:ext cx="7269120" cy="4388760"/>
+          <a:ext cx="7273800" cy="4388400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1343,23 +1361,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>618120</xdr:colOff>
+      <xdr:colOff>617760</xdr:colOff>
       <xdr:row>199</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Image 6" descr=""/>
+        <xdr:cNvPr id="25" name="Image 6" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27"/>
+        <a:blip r:embed="rId26"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604560" y="37335960"/>
-          <a:ext cx="9136440" cy="2241720"/>
+          <a:ext cx="9143640" cy="2241360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1380,23 +1398,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>194040</xdr:colOff>
       <xdr:row>243</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Image 10" descr=""/>
+        <xdr:cNvPr id="26" name="Image 10" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28"/>
+        <a:blip r:embed="rId27"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6604560" y="47111760"/>
-          <a:ext cx="7082280" cy="1526040"/>
+          <a:ext cx="7086960" cy="1525680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1417,23 +1435,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>352800</xdr:colOff>
+      <xdr:colOff>352440</xdr:colOff>
       <xdr:row>215</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Image 7" descr=""/>
+        <xdr:cNvPr id="27" name="Image 7" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29"/>
+        <a:blip r:embed="rId28"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6574680" y="40033440"/>
-          <a:ext cx="7270560" cy="2757600"/>
+          <a:ext cx="7275240" cy="2757240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1454,13 +1472,50 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>225360</xdr:colOff>
+      <xdr:colOff>225000</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Image 11" descr=""/>
+        <xdr:cNvPr id="28" name="Image 11" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId29"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604560" y="43035840"/>
+          <a:ext cx="7117920" cy="1908000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393840</xdr:colOff>
+      <xdr:row>266</xdr:row>
+      <xdr:rowOff>25560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Image 12" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1469,8 +1524,82 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6604560" y="43035840"/>
-          <a:ext cx="7113240" cy="1908360"/>
+          <a:off x="6604560" y="49087080"/>
+          <a:ext cx="7286760" cy="3807720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>545</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>207000</xdr:colOff>
+      <xdr:row>553</xdr:row>
+      <xdr:rowOff>64440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Image 14" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId31"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604560" y="107112240"/>
+          <a:ext cx="7099920" cy="1364760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>542</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>344520</xdr:colOff>
+      <xdr:row>544</xdr:row>
+      <xdr:rowOff>37440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Image 13" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId32"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6604560" y="106624440"/>
+          <a:ext cx="7237440" cy="362520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,13 +1619,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C524"/>
+  <dimension ref="A1:C543"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A209" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A226" activeCellId="0" sqref="A226"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A532" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C543" activeCellId="0" sqref="C543"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.7"/>
@@ -2581,12 +2710,8 @@
       <c r="B255" s="2"/>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B256" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A256" s="2"/>
+      <c r="B256" s="2"/>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2"/>
@@ -3675,6 +3800,75 @@
     <row r="524" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="4" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A527" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B527" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A529" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B529" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B532" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A534" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B534" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A536" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B536" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="538" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A538" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B538" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="540" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A540" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B540" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A543" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B543" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>